<commit_message>
Final Updated Edit Code
</commit_message>
<xml_diff>
--- a/Pivot Practice.xlsx
+++ b/Pivot Practice.xlsx
@@ -495,7 +495,7 @@
         <v>2019</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -512,7 +512,7 @@
         <v>2019</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -529,7 +529,7 @@
         <v>2019</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -648,7 +648,7 @@
         <v>2020</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -665,7 +665,7 @@
         <v>2020</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -682,7 +682,7 @@
         <v>2020</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -699,7 +699,7 @@
         <v>2020</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -716,7 +716,7 @@
         <v>2020</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -733,7 +733,7 @@
         <v>2020</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -852,7 +852,7 @@
         <v>2021</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -869,7 +869,7 @@
         <v>2021</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -886,7 +886,7 @@
         <v>2021</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -903,7 +903,7 @@
         <v>2021</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -920,7 +920,7 @@
         <v>2021</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -937,7 +937,7 @@
         <v>2021</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1056,7 +1056,7 @@
         <v>2022</v>
       </c>
       <c r="E38">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1073,7 +1073,7 @@
         <v>2022</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1090,7 +1090,7 @@
         <v>2022</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1107,7 +1107,7 @@
         <v>2022</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1124,7 +1124,7 @@
         <v>2022</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1141,7 +1141,7 @@
         <v>2022</v>
       </c>
       <c r="E43">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1260,7 +1260,7 @@
         <v>2023</v>
       </c>
       <c r="E50">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1277,7 +1277,7 @@
         <v>2023</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1294,7 +1294,7 @@
         <v>2023</v>
       </c>
       <c r="E52">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1311,7 +1311,7 @@
         <v>2023</v>
       </c>
       <c r="E53">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1328,7 +1328,7 @@
         <v>2023</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1345,7 +1345,7 @@
         <v>2023</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:5">

</xml_diff>

<commit_message>
Uploading final code without CSS
</commit_message>
<xml_diff>
--- a/Pivot Practice.xlsx
+++ b/Pivot Practice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="12">
   <si>
     <t>Country</t>
   </si>
@@ -407,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +495,7 @@
         <v>2019</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -512,7 +512,7 @@
         <v>2019</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -529,7 +529,7 @@
         <v>2019</v>
       </c>
       <c r="E7">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -648,7 +648,7 @@
         <v>2020</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -665,7 +665,7 @@
         <v>2020</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -682,7 +682,7 @@
         <v>2020</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -699,7 +699,7 @@
         <v>2020</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -716,7 +716,7 @@
         <v>2020</v>
       </c>
       <c r="E18">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -733,7 +733,7 @@
         <v>2020</v>
       </c>
       <c r="E19">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -852,7 +852,7 @@
         <v>2021</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -869,7 +869,7 @@
         <v>2021</v>
       </c>
       <c r="E27">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -886,7 +886,7 @@
         <v>2021</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -903,7 +903,7 @@
         <v>2021</v>
       </c>
       <c r="E29">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -920,7 +920,7 @@
         <v>2021</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -937,7 +937,7 @@
         <v>2021</v>
       </c>
       <c r="E31">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1056,7 +1056,7 @@
         <v>2022</v>
       </c>
       <c r="E38">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1073,7 +1073,7 @@
         <v>2022</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1090,7 +1090,7 @@
         <v>2022</v>
       </c>
       <c r="E40">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1107,7 +1107,7 @@
         <v>2022</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1124,7 +1124,7 @@
         <v>2022</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1141,7 +1141,7 @@
         <v>2022</v>
       </c>
       <c r="E43">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1260,7 +1260,7 @@
         <v>2023</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1277,7 +1277,7 @@
         <v>2023</v>
       </c>
       <c r="E51">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1294,7 +1294,7 @@
         <v>2023</v>
       </c>
       <c r="E52">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1311,7 +1311,7 @@
         <v>2023</v>
       </c>
       <c r="E53">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1328,7 +1328,7 @@
         <v>2023</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1345,7 +1345,7 @@
         <v>2023</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1447,6 +1447,786 @@
         <v>2023</v>
       </c>
       <c r="E61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62">
+        <v>2024</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>2024</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64">
+        <v>2024</v>
+      </c>
+      <c r="E64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <v>2024</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>2024</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>2024</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>2024</v>
+      </c>
+      <c r="E68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>2024</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>2024</v>
+      </c>
+      <c r="E70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71">
+        <v>2024</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>2024</v>
+      </c>
+      <c r="E72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73">
+        <v>2024</v>
+      </c>
+      <c r="E73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74">
+        <v>2025</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>2025</v>
+      </c>
+      <c r="E75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76">
+        <v>2025</v>
+      </c>
+      <c r="E76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>2025</v>
+      </c>
+      <c r="E77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>2025</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79">
+        <v>2025</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80">
+        <v>2025</v>
+      </c>
+      <c r="E80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>2025</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82">
+        <v>2025</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>2025</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>2025</v>
+      </c>
+      <c r="E84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85">
+        <v>2025</v>
+      </c>
+      <c r="E85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98">
+        <v>2026</v>
+      </c>
+      <c r="E98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>2026</v>
+      </c>
+      <c r="E99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100">
+        <v>2026</v>
+      </c>
+      <c r="E100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101">
+        <v>2026</v>
+      </c>
+      <c r="E101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>2026</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103">
+        <v>2026</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104">
+        <v>2026</v>
+      </c>
+      <c r="E104">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105">
+        <v>2026</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106">
+        <v>2026</v>
+      </c>
+      <c r="E106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107">
+        <v>2026</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108">
+        <v>2026</v>
+      </c>
+      <c r="E108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109">
+        <v>2026</v>
+      </c>
+      <c r="E109">
         <v>7</v>
       </c>
     </row>

</xml_diff>